<commit_message>
switched to yahoo finance
</commit_message>
<xml_diff>
--- a/Holdings.xlsx
+++ b/Holdings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sumeetvaidya/bootcamp-project-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D5B592-C89A-5944-A516-B977174C44F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FC6C58-D0D6-1C49-9736-88C860521B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16040" xr2:uid="{D75FB4D3-98EB-FF4C-9B8F-EE8E706021A6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Acquisition Date</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>TWTR</t>
+  </si>
+  <si>
+    <t>TTD</t>
   </si>
 </sst>
 </file>
@@ -472,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A65DF8-7C5F-E640-9674-8A512B0F279D}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,14 +514,14 @@
         <v>6</v>
       </c>
       <c r="C2" s="4">
-        <v>125</v>
+        <v>300</v>
       </c>
       <c r="D2" s="5">
         <v>43.5</v>
       </c>
       <c r="E2" s="6">
         <f>+C2*D2</f>
-        <v>5437.5</v>
+        <v>13050</v>
       </c>
       <c r="F2" s="2">
         <v>44196</v>
@@ -538,7 +541,7 @@
         <v>132.5</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" ref="E3:E9" si="0">+C3*D3</f>
+        <f t="shared" ref="E3:E10" si="0">+C3*D3</f>
         <v>13250</v>
       </c>
       <c r="F3" s="2">
@@ -574,14 +577,14 @@
         <v>9</v>
       </c>
       <c r="C5" s="4">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="D5" s="7">
         <v>55.8</v>
       </c>
       <c r="E5" s="6">
         <f t="shared" si="0"/>
-        <v>33480</v>
+        <v>11160</v>
       </c>
       <c r="F5" s="2">
         <v>44196</v>
@@ -668,6 +671,27 @@
         <v>6819.75</v>
       </c>
       <c r="F9" s="2">
+        <v>44196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>43503</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4">
+        <v>100</v>
+      </c>
+      <c r="D10" s="7">
+        <v>14.3</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="0"/>
+        <v>1430</v>
+      </c>
+      <c r="F10" s="2">
         <v>44196</v>
       </c>
     </row>

</xml_diff>